<commit_message>
Incluido comprobar compatibilidad wcag sobre ficheros en bruto, se ha incluido en la base de datos la tabla ficheros para gestionarlos y distintas funciones asociadas a esta tabla en el módulo y en los test
</commit_message>
<xml_diff>
--- a/data/formatted/Datos WCAG Ayuntamientos - copia_formatted.xlsx
+++ b/data/formatted/Datos WCAG Ayuntamientos - copia_formatted.xlsx
@@ -5504,7 +5504,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3.5 Identify Input Purpose</t>
+          <t>1.3.6 Identify Purpose</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">1.3.6 Identify Purpose </t>
+          <t>1.3.6 Identify Purpose</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -15341,7 +15341,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2.4.4: Link Purpose (In Context)</t>
+          <t>2.4.9: Link Purpose (Link Only)</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -21998,7 +21998,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>3.2.3: Consistent Navigation</t>
+          <t>3.2.4: Consistent Identification</t>
         </is>
       </c>
       <c r="D82" t="n">

</xml_diff>

<commit_message>
Mejoras para filtrar por versión, se mueven funciones de gestion al módulo de wcag
</commit_message>
<xml_diff>
--- a/data/formatted/Datos WCAG Ayuntamientos - copia_formatted.xlsx
+++ b/data/formatted/Datos WCAG Ayuntamientos - copia_formatted.xlsx
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1.1: Non-text Content</t>
+          <t>1.1.1 Non-text Content</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2.1: Audio-only and Video-only (Prerecorded)</t>
+          <t>1.2.1 Audio-only and Video-only (Prerecorded)</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2.2: Captions (Prerecorded)</t>
+          <t>1.2.2 Captions (Prerecorded)</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2.3: Audio Description or Media Alternative (Prerecorded)</t>
+          <t>1.2.3 Audio Description or Media Alternative (Prerecorded)</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2.4: Captions (Live)</t>
+          <t>1.2.4 Captions (Live)</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2.5: Audio Description (Prerecorded)</t>
+          <t>1.2.5 Audio Description (Prerecorded)</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.2.8  Media Alternative (Prerecorded)</t>
+          <t>1.2.8 Media Alternative (Prerecorded)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3.1: Info and Relationships</t>
+          <t>1.3.1 Info and Relationships</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3.2: Meaningful Sequence</t>
+          <t>1.3.2 Meaningful Sequence</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -4910,7 +4910,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3.3: Sensory Characteristics</t>
+          <t>1.3.3 Sensory Characteristics</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -5504,7 +5504,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3.6 Identify Purpose</t>
+          <t>1.3.5 Identify Input Purpose</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.4.1: Use of Color</t>
+          <t>1.4.1 Use of Color</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.4.2: Audio Control</t>
+          <t>1.4.2 Audio Control</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -6797,7 +6797,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4.3: Contrast (Minimum)</t>
+          <t>1.4.3 Contrast (Minimum)</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -7094,7 +7094,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.4.4: Resize text</t>
+          <t>1.4.4 Resize text</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -7391,7 +7391,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.4.5: Images of Text</t>
+          <t>1.4.5 Images of Text</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -7688,7 +7688,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.4.6: Contrast (Enhanced)</t>
+          <t>1.4.6 Contrast (Enhanced)</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -7985,7 +7985,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.4.7: Low or No Background audio</t>
+          <t>1.4.7 Low or No Background audio</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -8282,7 +8282,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4.8: Visual Presentation</t>
+          <t>1.4.8 Visual Presentation</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -8579,7 +8579,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.4.9: Images of Text (No Exception)</t>
+          <t>1.4.9 Images of Text (No Exception)</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">1.4.12 Text Spacing </t>
+          <t>1.4.12 Text Spacing</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -10274,7 +10274,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2.1.1: Keyboard</t>
+          <t>2.1.1 Keyboard</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -10571,7 +10571,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.1.2: No Keyboard Trap</t>
+          <t>2.1.2 No Keyboard Trap</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -11567,7 +11567,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2.2.1: Timing Adjustable</t>
+          <t>2.2.1 Timing Adjustable</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -11864,7 +11864,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2.2.2: Pause, Stop, Hide</t>
+          <t>2.2.2 Pause, Stop, Hide</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -12161,7 +12161,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2.2.3: No Timing</t>
+          <t>2.2.3 No Timing</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2.2.4: Interruptions</t>
+          <t>2.2.4 Interruptions</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -12755,7 +12755,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2.2.5: Re-authenticating</t>
+          <t>2.2.5 Re-authenticating</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -13052,7 +13052,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">2.2.6 Timeouts </t>
+          <t>2.2.6 Timeouts</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -13454,7 +13454,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2.3.1: Three Flashes or Below Threshold</t>
+          <t>2.3.1 Three Flashes or Below Threshold</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -13751,7 +13751,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2.3.2: Three Flashes</t>
+          <t>2.3.2 Three Flashes</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -14450,7 +14450,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2.4.1: Bypass Blocks</t>
+          <t>2.4.1 Bypass Blocks</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -14747,7 +14747,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2.4.2: Page Titled</t>
+          <t>2.4.2 Page Titled</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -15044,7 +15044,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2.4.3: Focus Order</t>
+          <t>2.4.3 Focus Order</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -15341,7 +15341,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2.4.9: Link Purpose (Link Only)</t>
+          <t>2.4.4 Link Purpose (In Context)</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -15638,7 +15638,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2.4.5: Multiple Ways</t>
+          <t>2.4.5 Multiple Ways</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.4.6: Headings and Labels</t>
+          <t>2.4.6 Headings and Labels</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -16232,7 +16232,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2.4.7: Focus Visible</t>
+          <t>2.4.7 Focus Visible</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -16529,7 +16529,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2.4.8: Location</t>
+          <t>2.4.8 Location</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -16826,7 +16826,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2.4.9: Link Purpose (Link Only)</t>
+          <t>2.4.9 Link Purpose (Link Only)</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -17123,7 +17123,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2.4.10: Section Headings</t>
+          <t>2.4.10 Section Headings</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -19517,7 +19517,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>3.1.1: Language of Page</t>
+          <t>3.1.1 Language of Page</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -19814,7 +19814,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>3.1.2: Language of Parts</t>
+          <t>3.1.2 Language of Parts</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -20111,7 +20111,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>3.1.3: Unusual Words</t>
+          <t>3.1.3 Unusual Words</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -20408,7 +20408,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>3.1.4: Abbreviations</t>
+          <t>3.1.4 Abbreviations</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -21002,7 +21002,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>3.1.6: Pronunciation</t>
+          <t>3.1.6 Pronunciation</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -21404,7 +21404,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>3.2.1: On Focus</t>
+          <t>3.2.1 On Focus</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -21701,7 +21701,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>3.2.2: On Input</t>
+          <t>3.2.2 On Input</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -21998,7 +21998,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>3.2.4: Consistent Identification</t>
+          <t>3.2.3 Consistent Navigation</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -22295,7 +22295,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>3.2.4: Consistent Identification</t>
+          <t>3.2.4 Consistent Identification</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -22592,7 +22592,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>3.2.5: Change in Request</t>
+          <t>3.2.5 Change in Request</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -22994,7 +22994,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>3.3.1: Error Identification</t>
+          <t>3.3.1 Error Identification</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -23291,7 +23291,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>3.3.2: Labels or Instructions</t>
+          <t>3.3.2 Labels or Instructions</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -23588,7 +23588,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>3.3.3: Error Suggestion</t>
+          <t>3.3.3 Error Suggestion</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -23885,7 +23885,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>3.3.4: Error Prevention (Legal, Financial, Data)</t>
+          <t>3.3.4 Error Prevention (Legal, Financial, Data)</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -24182,7 +24182,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>3.3.5: Help</t>
+          <t>3.3.5 Help</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -24479,7 +24479,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>3.3.6: Error Prevention (All)</t>
+          <t>3.3.6 Error Prevention (All)</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -24986,7 +24986,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>4.1.1: Parsing(Obsolete and removed)</t>
+          <t>4.1.1 Parsing(Obsolete and removed)</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -25283,7 +25283,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>4.1.2: Name, Role, Value</t>
+          <t>4.1.2 Name, Role, Value</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">4.1.3 Status Messages </t>
+          <t>4.1.3 Status Messages</t>
         </is>
       </c>
       <c r="D96" t="n">

</xml_diff>